<commit_message>
feat: excel, planilha counts ::by sergio giraldo @ 20250522T1353CEST, gpg signed
</commit_message>
<xml_diff>
--- a/excel/counts.xlsx
+++ b/excel/counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8EEE70-BA21-4F4B-BD31-9F3C0EF63718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A5E057-5B60-904D-BE91-70A3F7989EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{20C0F889-BAB8-481D-82E6-B0D0A3AF10F9}"/>
   </bookViews>
@@ -16,6 +16,40 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="CONSOLIDATED" sheetId="6" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">CONSOLIDATED!$A$6:$A$12</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">CONSOLIDATED!$B$5</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">CONSOLIDATED!$F$6:$F$12</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">CONSOLIDATED!$G$5</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">CONSOLIDATED!$G$6:$G$12</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">CONSOLIDATED!$H$5</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">CONSOLIDATED!$H$6:$H$12</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">CONSOLIDATED!$I$5</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">CONSOLIDATED!$I$6:$I$12</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">CONSOLIDATED!$A$10</definedName>
+    <definedName name="_xlchart.v2.18" hidden="1">CONSOLIDATED!$A$11</definedName>
+    <definedName name="_xlchart.v2.19" hidden="1">CONSOLIDATED!$A$12</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">CONSOLIDATED!$B$6:$B$12</definedName>
+    <definedName name="_xlchart.v2.20" hidden="1">CONSOLIDATED!$A$6</definedName>
+    <definedName name="_xlchart.v2.21" hidden="1">CONSOLIDATED!$A$7</definedName>
+    <definedName name="_xlchart.v2.22" hidden="1">CONSOLIDATED!$A$8</definedName>
+    <definedName name="_xlchart.v2.23" hidden="1">CONSOLIDATED!$A$9</definedName>
+    <definedName name="_xlchart.v2.24" hidden="1">CONSOLIDATED!$B$10:$I$10</definedName>
+    <definedName name="_xlchart.v2.25" hidden="1">CONSOLIDATED!$B$11:$I$11</definedName>
+    <definedName name="_xlchart.v2.26" hidden="1">CONSOLIDATED!$B$12:$I$12</definedName>
+    <definedName name="_xlchart.v2.27" hidden="1">CONSOLIDATED!$B$5:$I$5</definedName>
+    <definedName name="_xlchart.v2.28" hidden="1">CONSOLIDATED!$B$6:$I$6</definedName>
+    <definedName name="_xlchart.v2.29" hidden="1">CONSOLIDATED!$B$7:$I$7</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">CONSOLIDATED!$C$5</definedName>
+    <definedName name="_xlchart.v2.30" hidden="1">CONSOLIDATED!$B$8:$I$8</definedName>
+    <definedName name="_xlchart.v2.31" hidden="1">CONSOLIDATED!$B$9:$I$9</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">CONSOLIDATED!$C$6:$C$12</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">CONSOLIDATED!$D$5</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">CONSOLIDATED!$D$6:$D$12</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">CONSOLIDATED!$E$5</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">CONSOLIDATED!$E$6:$E$12</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">CONSOLIDATED!$F$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>AZURE</t>
   </si>
@@ -167,6 +201,12 @@
   </si>
   <si>
     <t>tudo e dinamico, ate as bordas, unica coisa para isto funcionar eh manter o nome da planilha como sheet 1. as formulas estao entre as celulas A5 e AD50. As bordas usam conditional formatting</t>
+  </si>
+  <si>
+    <t>JOY</t>
+  </si>
+  <si>
+    <t>foo12</t>
   </si>
 </sst>
 </file>
@@ -290,25 +330,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <border>
         <left style="thin">
@@ -722,7 +744,7 @@
   <dimension ref="A1:CN42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -983,8 +1005,19 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:92" ht="21" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="P13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="P13" ca="1">IF(INDIRECT(ADDRESS(12,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT(LEFT(ADDRESS(1,MATCH(CONSOLIDATED!$A6,$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH(CONSOLIDATED!$A6,$1:$1,0),4),1)),"X",$A:$A,P$12),"")</f>
@@ -2646,7 +2679,7 @@
   <dimension ref="A1:AD60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AD3"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2723,7 +2756,7 @@
     <row r="5" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="10" t="str" cm="1">
-        <f t="array" ref="B5:H5">TRANSPOSE(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Sheet1!A2:A10000,Sheet1!A2:A10000&lt;&gt;"")))</f>
+        <f t="array" ref="B5:I5">TRANSPOSE(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Sheet1!A2:A10000,Sheet1!A2:A10000&lt;&gt;"")))</f>
         <v>JOHN</v>
       </c>
       <c r="C5" s="10" t="str">
@@ -2744,7 +2777,9 @@
       <c r="H5" s="10" t="str">
         <v>JACK</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="str">
+        <v>JOY</v>
+      </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -2800,9 +2835,9 @@
         <f t="array" aca="1" ref="H6" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>0</v>
       </c>
-      <c r="I6" s="12" t="str" cm="1">
+      <c r="I6" s="12" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J6" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A6,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -2921,9 +2956,9 @@
         <f t="array" aca="1" ref="H7" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>0</v>
       </c>
-      <c r="I7" s="12" t="str" cm="1">
+      <c r="I7" s="12" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J7" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A7,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -3042,9 +3077,9 @@
         <f t="array" aca="1" ref="H8" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>0</v>
       </c>
-      <c r="I8" s="12" t="str" cm="1">
+      <c r="I8" s="12" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J8" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A8,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -3163,9 +3198,9 @@
         <f t="array" aca="1" ref="H9" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>1</v>
       </c>
-      <c r="I9" s="12" t="str" cm="1">
+      <c r="I9" s="12" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J9" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A9,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -3284,9 +3319,9 @@
         <f t="array" aca="1" ref="H10" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>1</v>
       </c>
-      <c r="I10" s="12" t="str" cm="1">
+      <c r="I10" s="12" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J10" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A10,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -3405,9 +3440,9 @@
         <f t="array" aca="1" ref="H11" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>1</v>
       </c>
-      <c r="I11" s="12" t="str" cm="1">
+      <c r="I11" s="12" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J11" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A11,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -3526,9 +3561,9 @@
         <f t="array" aca="1" ref="H12" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),""),"")</f>
         <v>1</v>
       </c>
-      <c r="I12" s="12" t="str" cm="1">
+      <c r="I12" s="12" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),""),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J12" s="12" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",IF(INDIRECT(ADDRESS(ROW(),1))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A12,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),""),"")</f>
@@ -8524,9 +8559,9 @@
         <f t="array" aca="1" ref="H54" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),"")</f>
         <v>#N/A</v>
       </c>
-      <c r="I54" s="5" t="str" cm="1">
+      <c r="I54" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="I54" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),"")</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="J54" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="J54" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A54,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),"")</f>
@@ -8643,9 +8678,9 @@
         <f t="array" aca="1" ref="H55" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),"")</f>
         <v>#N/A</v>
       </c>
-      <c r="I55" s="5" t="str" cm="1">
+      <c r="I55" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="I55" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),"")</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="J55" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="J55" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A55,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),"")</f>
@@ -8762,9 +8797,9 @@
         <f t="array" aca="1" ref="H56" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),"")</f>
         <v>#N/A</v>
       </c>
-      <c r="I56" s="5" t="str" cm="1">
+      <c r="I56" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="I56" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),"")</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="J56" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="J56" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A56,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),"")</f>
@@ -8881,9 +8916,9 @@
         <f t="array" aca="1" ref="H57" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,H$5),"")</f>
         <v>#N/A</v>
       </c>
-      <c r="I57" s="5" t="str" cm="1">
+      <c r="I57" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="I57" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,I$5),"")</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="J57" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="J57" ca="1">IF(INDIRECT(ADDRESS(5,COLUMN()))&amp;""&lt;&gt;"",COUNTIFS(INDIRECT("Sheet1!"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)&amp;":"&amp;LEFT(ADDRESS(1,MATCH($A57,Sheet1!$1:$1,0),4),1)),"X",Sheet1!$A:$A,J$5),"")</f>

</xml_diff>